<commit_message>
bulk orders updated. Place Customer orders. Checkout.
</commit_message>
<xml_diff>
--- a/adminDashboard/files/bulkOrders.xlsx
+++ b/adminDashboard/files/bulkOrders.xlsx
@@ -20,9 +20,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t xml:space="preserve">ProductId</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+  <si>
+    <t xml:space="preserve">ItemCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ItemName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Itemtype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FamilyCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FamilyDesc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isactive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WeightUoM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Itemgroup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GroupDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ModelNumber </t>
   </si>
   <si>
     <t xml:space="preserve">Quantity</t>
@@ -31,7 +61,25 @@
     <t xml:space="preserve">levas123</t>
   </si>
   <si>
+    <t xml:space="preserve">Leva S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Machine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commercial Machine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grams</t>
+  </si>
+  <si>
     <t xml:space="preserve">lineamini123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linea Mini</t>
   </si>
 </sst>
 </file>
@@ -41,7 +89,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -62,6 +110,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -73,8 +128,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFCCFFCC"/>
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -124,8 +179,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -144,7 +199,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFEEEEEE"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -166,7 +221,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -209,13 +264,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="14.8469387755102"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -224,20 +288,100 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>2</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>4500</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="2" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Header for moble view added in landing page
</commit_message>
<xml_diff>
--- a/adminDashboard/files/bulkOrders.xlsx
+++ b/adminDashboard/files/bulkOrders.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -214,7 +214,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -299,19 +299,19 @@
   </sheetPr>
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="9.14"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.9878542510121"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.46153846153846"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -430,7 +430,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>18</v>
@@ -530,7 +530,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>28</v>
@@ -650,7 +650,7 @@
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>40</v>
@@ -1220,7 +1220,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>